<commit_message>
adding PTC_N and ITC_N to ALEAF_Master_LC_GEP
</commit_message>
<xml_diff>
--- a/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP.xlsx
+++ b/inputs/ALEAF_inputs/ALEAF_Master_LC_GEP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\biegelk\abce\inputs\ALEAF_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E30200-2A39-414E-AC96-16E6B933B96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{336AED84-67D2-493B-B9E4-C82E0AA31C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" tabRatio="927" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="305">
   <si>
     <t>NDAYS</t>
   </si>
@@ -995,6 +995,12 @@
   </si>
   <si>
     <t>AdvancedNuclear</t>
+  </si>
+  <si>
+    <t>PTC_N</t>
+  </si>
+  <si>
+    <t>ITC_N</t>
   </si>
 </sst>
 </file>
@@ -1444,6 +1450,156 @@
   </cellStyles>
   <dxfs count="32">
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1730,156 +1886,6 @@
         </bottom>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1894,21 +1900,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C398F006-9176-439E-89B4-C1E7E01F4A75}" name="Table15" displayName="Table15" ref="A1:M29" totalsRowShown="0" dataDxfId="15" headerRowBorderDxfId="16" headerRowCellStyle="Heading 3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{C398F006-9176-439E-89B4-C1E7E01F4A75}" name="Table15" displayName="Table15" ref="A1:M29" totalsRowShown="0" dataDxfId="30" headerRowBorderDxfId="31" headerRowCellStyle="Heading 3">
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{3DC2679D-B62E-4882-96BC-E061D16C80E3}" name="ATB_Setting_ID" dataDxfId="14" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="2" xr3:uid="{1CAA5CEC-F6C3-4266-B10F-5D8DCF3D9F6B}" name="Tech_ID" dataDxfId="13" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="3" xr3:uid="{0498CE57-061B-4656-B978-EE3D71710707}" name="UNITGROUP" dataDxfId="12" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="4" xr3:uid="{9AC12795-D144-4EE8-A5B6-1176B6F8D41C}" name="UNIT_CATEGORY" dataDxfId="11" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="5" xr3:uid="{37C07C8E-4FC1-49A2-982B-7BBA5F026E01}" name="UNIT_TYPE" dataDxfId="10" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="6" xr3:uid="{04CAEE9C-06F8-4B70-B3F4-47E02C7259F3}" name="FUEL" dataDxfId="9" dataCellStyle="20% - Accent4"/>
-    <tableColumn id="7" xr3:uid="{9EFCD535-F1B6-4D50-8FB1-DE0BDDF09E86}" name="Tech" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{E1998447-7307-42A6-B0F4-1AD822918E38}" name="TechDetail" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{2261B3A3-876C-40DE-8E99-04E71CEEBD51}" name="Case" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{0F4D500B-389E-459E-B02B-79B416977956}" name="CRP" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{3AA769FF-EAA2-49EC-A32C-1E4BE22E2E2B}" name="Scenario" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{0EEEA7F5-755D-4DE9-8AFD-B691AB0EF5D1}" name="Year" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{B85F03DA-4DAB-4815-8190-4094A98EE221}" name="ATB Year" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3DC2679D-B62E-4882-96BC-E061D16C80E3}" name="ATB_Setting_ID" dataDxfId="29" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="2" xr3:uid="{1CAA5CEC-F6C3-4266-B10F-5D8DCF3D9F6B}" name="Tech_ID" dataDxfId="28" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="3" xr3:uid="{0498CE57-061B-4656-B978-EE3D71710707}" name="UNITGROUP" dataDxfId="27" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="4" xr3:uid="{9AC12795-D144-4EE8-A5B6-1176B6F8D41C}" name="UNIT_CATEGORY" dataDxfId="26" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="5" xr3:uid="{37C07C8E-4FC1-49A2-982B-7BBA5F026E01}" name="UNIT_TYPE" dataDxfId="25" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="6" xr3:uid="{04CAEE9C-06F8-4B70-B3F4-47E02C7259F3}" name="FUEL" dataDxfId="24" dataCellStyle="20% - Accent4"/>
+    <tableColumn id="7" xr3:uid="{9EFCD535-F1B6-4D50-8FB1-DE0BDDF09E86}" name="Tech" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{E1998447-7307-42A6-B0F4-1AD822918E38}" name="TechDetail" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{2261B3A3-876C-40DE-8E99-04E71CEEBD51}" name="Case" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{0F4D500B-389E-459E-B02B-79B416977956}" name="CRP" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{3AA769FF-EAA2-49EC-A32C-1E4BE22E2E2B}" name="Scenario" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{0EEEA7F5-755D-4DE9-8AFD-B691AB0EF5D1}" name="Year" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{B85F03DA-4DAB-4815-8190-4094A98EE221}" name="ATB Year" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1997,10 +2003,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{666EA2BE-3015-409E-80D7-7F92F88651B9}" name="Table2" displayName="Table2" ref="I1:I6" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{666EA2BE-3015-409E-80D7-7F92F88651B9}" name="Table2" displayName="Table2" ref="I1:I6" totalsRowShown="0" dataDxfId="16">
   <autoFilter ref="I1:I6" xr:uid="{4FFF85DB-E87B-497F-961E-2FB45C949196}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{360A7678-57E4-403D-8CD3-9F511FAEF1F4}" name="Battery" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{360A7678-57E4-403D-8CD3-9F511FAEF1F4}" name="Battery" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5782,10 +5788,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5584FCC-2587-4776-A2D1-EC36BF3CF093}">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25"/>
@@ -5800,7 +5806,7 @@
     <col min="24" max="24" width="9.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="22" customFormat="1" ht="14.65" thickBot="1">
+    <row r="1" spans="1:26" s="22" customFormat="1" ht="14.65" thickBot="1">
       <c r="A1" s="18" t="s">
         <v>99</v>
       </c>
@@ -5870,11 +5876,17 @@
       <c r="W1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="18" t="s">
+      <c r="X1" s="22" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y1" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="Z1" s="18" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:26">
       <c r="A2" t="s">
         <v>292</v>
       </c>
@@ -5945,6 +5957,12 @@
         <v>0</v>
       </c>
       <c r="X2" s="41">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="41">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="41">
         <v>0</v>
       </c>
     </row>
@@ -6885,7 +6903,7 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="AJ2:AJ8">
-    <cfRule type="cellIs" dxfId="31" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="45" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="46">
@@ -6900,7 +6918,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK2:AK5">
-    <cfRule type="cellIs" dxfId="30" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="43" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="44">
@@ -6915,7 +6933,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK6:AK8">
-    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="25" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="26">
@@ -6930,7 +6948,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH2">
-    <cfRule type="cellIs" dxfId="28" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="16">
@@ -6945,7 +6963,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH3">
-    <cfRule type="cellIs" dxfId="27" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="14">
@@ -6960,7 +6978,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI2:AI3">
-    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="18">
@@ -6975,7 +6993,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH5:AH7">
-    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="20">
@@ -6990,7 +7008,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI5:AI7">
-    <cfRule type="cellIs" dxfId="24" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="21" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="22">
@@ -7005,7 +7023,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD2:AF2 AE5:AF7 AE3:AF3 AD3:AD8">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="23" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="24">
@@ -7020,7 +7038,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH4">
-    <cfRule type="cellIs" dxfId="22" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="10">
@@ -7035,7 +7053,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI4">
-    <cfRule type="cellIs" dxfId="21" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="8">
@@ -7050,7 +7068,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE4:AF4">
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="12">
@@ -7065,7 +7083,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH8">
-    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -7080,7 +7098,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI8">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="4">
@@ -7095,7 +7113,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE8:AF8">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
     <cfRule type="colorScale" priority="6">

</xml_diff>